<commit_message>
Generalized load_excel_sheet from Utilities
</commit_message>
<xml_diff>
--- a/Tom/AOOrderHistory.xlsx
+++ b/Tom/AOOrderHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ScrumbagsRepos\AO-Responsiveness-Testing\Tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259319C2-84AD-4A59-9A90-38D62EDF58AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12A2DA6-0EB3-4D89-B3DC-73EF760713BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D8DC93A-2799-4B4D-A332-7A5BE98C1B10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>DT_email</t>
   </si>
@@ -48,13 +48,25 @@
   </si>
   <si>
     <t>Testing123!</t>
+  </si>
+  <si>
+    <t>TH_TC014</t>
+  </si>
+  <si>
+    <t>TH_TC014_R</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>test9183</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +79,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,10 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,31 +429,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F5691C-CA72-4969-98DD-A66C03071613}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Had to add new orders as AO wiped order history
</commit_message>
<xml_diff>
--- a/Tom/AOOrderHistory.xlsx
+++ b/Tom/AOOrderHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ScrumbagsRepos\AO-Responsiveness-Testing\Tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88988A81-1E9D-4651-B604-60508F6EB4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED1A55B-F88E-4816-98A4-7716D214C996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13845" yWindow="-14430" windowWidth="11235" windowHeight="13080" xr2:uid="{8D8DC93A-2799-4B4D-A332-7A5BE98C1B10}"/>
+    <workbookView xWindow="9075" yWindow="-14190" windowWidth="16635" windowHeight="13080" xr2:uid="{8D8DC93A-2799-4B4D-A332-7A5BE98C1B10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>DT_email</t>
   </si>
@@ -50,13 +50,79 @@
     <t>Testing123!</t>
   </si>
   <si>
-    <t>TH_TC014</t>
-  </si>
-  <si>
-    <t>TH_TC014_R</t>
-  </si>
-  <si>
     <t>TC</t>
+  </si>
+  <si>
+    <t>DT_order_number</t>
+  </si>
+  <si>
+    <t>DT_order_date</t>
+  </si>
+  <si>
+    <t>DT_order_time</t>
+  </si>
+  <si>
+    <t>DT_product_name</t>
+  </si>
+  <si>
+    <t>DT_quantity</t>
+  </si>
+  <si>
+    <t>DT_total_price</t>
+  </si>
+  <si>
+    <t>Bose Soundlink Bluetooth Speaker III</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>$269.99</t>
+  </si>
+  <si>
+    <t>TH_TC014_1</t>
+  </si>
+  <si>
+    <t>HP ElitePad 1000 G2 Tablet</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>$2,018.00</t>
+  </si>
+  <si>
+    <t>TH_TC014_2</t>
+  </si>
+  <si>
+    <t>TH_TC014_3</t>
+  </si>
+  <si>
+    <t>$569.98</t>
+  </si>
+  <si>
+    <t>4989273967</t>
+  </si>
+  <si>
+    <t>06/10/2022</t>
+  </si>
+  <si>
+    <t>9:13:59 AM</t>
+  </si>
+  <si>
+    <t>4989275115</t>
+  </si>
+  <si>
+    <t>9:14:23 AM</t>
+  </si>
+  <si>
+    <t>9:14:10 AM</t>
+  </si>
+  <si>
+    <t>4989273968</t>
+  </si>
+  <si>
+    <t>Beats Studio 2 Over-Ear Matte Black Headphones</t>
   </si>
 </sst>
 </file>
@@ -107,11 +173,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,21 +491,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F5691C-CA72-4969-98DD-A66C03071613}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="14" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>6</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -448,10 +519,28 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -459,10 +548,28 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -470,7 +577,55 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added separate sheet for TH_TC015
</commit_message>
<xml_diff>
--- a/Tom/AOOrderHistory.xlsx
+++ b/Tom/AOOrderHistory.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ScrumbagsRepos\AO-Responsiveness-Testing\Tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED1A55B-F88E-4816-98A4-7716D214C996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63514CEA-EEA3-44F1-A8CC-60F7581C9B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9075" yWindow="-14190" windowWidth="16635" windowHeight="13080" xr2:uid="{8D8DC93A-2799-4B4D-A332-7A5BE98C1B10}"/>
+    <workbookView xWindow="5745" yWindow="2340" windowWidth="16635" windowHeight="13080" activeTab="1" xr2:uid="{8D8DC93A-2799-4B4D-A332-7A5BE98C1B10}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TH_TC014" sheetId="1" r:id="rId1"/>
+    <sheet name="TH_TC015" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>DT_email</t>
   </si>
@@ -53,6 +54,9 @@
     <t>TC</t>
   </si>
   <si>
+    <t>test9183</t>
+  </si>
+  <si>
     <t>DT_order_number</t>
   </si>
   <si>
@@ -98,9 +102,6 @@
     <t>TH_TC014_3</t>
   </si>
   <si>
-    <t>$569.98</t>
-  </si>
-  <si>
     <t>4989273967</t>
   </si>
   <si>
@@ -123,6 +124,12 @@
   </si>
   <si>
     <t>Beats Studio 2 Over-Ear Matte Black Headphones</t>
+  </si>
+  <si>
+    <t>$189.98</t>
+  </si>
+  <si>
+    <t>TH_TC015_1</t>
   </si>
 </sst>
 </file>
@@ -493,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F5691C-CA72-4969-98DD-A66C03071613}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,27 +527,27 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -558,18 +565,18 @@
         <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -587,18 +594,18 @@
         <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
@@ -619,10 +626,10 @@
         <v>28</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -631,4 +638,44 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0548339-D866-4A48-B313-875EDFC0E048}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final version - added tablet tests
</commit_message>
<xml_diff>
--- a/Tom/AOOrderHistory.xlsx
+++ b/Tom/AOOrderHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ScrumbagsRepos\AO-Responsiveness-Testing\Tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63514CEA-EEA3-44F1-A8CC-60F7581C9B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CDC1E7-406C-4227-862A-57BBACC1E50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5745" yWindow="2340" windowWidth="16635" windowHeight="13080" activeTab="1" xr2:uid="{8D8DC93A-2799-4B4D-A332-7A5BE98C1B10}"/>
+    <workbookView xWindow="6585" yWindow="2760" windowWidth="21600" windowHeight="11295" xr2:uid="{8D8DC93A-2799-4B4D-A332-7A5BE98C1B10}"/>
   </bookViews>
   <sheets>
     <sheet name="TH_TC014" sheetId="1" r:id="rId1"/>
@@ -108,18 +108,9 @@
     <t>06/10/2022</t>
   </si>
   <si>
-    <t>9:13:59 AM</t>
-  </si>
-  <si>
     <t>4989275115</t>
   </si>
   <si>
-    <t>9:14:23 AM</t>
-  </si>
-  <si>
-    <t>9:14:10 AM</t>
-  </si>
-  <si>
     <t>4989273968</t>
   </si>
   <si>
@@ -130,6 +121,15 @@
   </si>
   <si>
     <t>TH_TC015_1</t>
+  </si>
+  <si>
+    <t>10:13:59 AM</t>
+  </si>
+  <si>
+    <t>10:14:10 AM</t>
+  </si>
+  <si>
+    <t>10:14:23 AM</t>
   </si>
 </sst>
 </file>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F5691C-CA72-4969-98DD-A66C03071613}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +562,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>12</v>
@@ -585,13 +585,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
@@ -614,22 +614,22 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -644,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0548339-D866-4A48-B313-875EDFC0E048}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -666,7 +666,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>

</xml_diff>